<commit_message>
inital chat updated with explaination of the WVS and the core value/qualities
</commit_message>
<xml_diff>
--- a/data/describe/Core_values.xlsx
+++ b/data/describe/Core_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Desktop\Green_Git\twelve-gpt-educational\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAC9EBB-14C4-4E47-859D-00099B9C869E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1726C17E-6397-4468-BB71-588EFDF4455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>user</t>
   </si>
@@ -28,21 +28,114 @@
     <t>assistant</t>
   </si>
   <si>
-    <t>What is a core value?</t>
+    <t>What is the World Value Survey?</t>
   </si>
   <si>
-    <t xml:space="preserve">A core value is a fundamental belief or principle that guides behavior, decision-making, and actions. It serves as a foundational element of an individual’s or organization's identity, often reflecting their priorities, ethics, and goals. </t>
+    <t>The World Values Survey is an international research program devoted to the scientific and academic study of social, political, economic, religious and cultural values of people in the world. The project’s goal is to assess which impact values stability or change over time has on the social, political and economic development of countries and societies.</t>
+  </si>
+  <si>
+    <t>How is the World Value Survey conducted?</t>
+  </si>
+  <si>
+    <t>The World Value Survey (WVS) consists of nationally representative surveys conducted in almost 100 countries which contain almost 90 percent of the world’s population, using a common questionnaire. The WVS is the largest non-commercial, cross-national, time series investigation of human beliefs and values ever executed, currently including interviews with almost 400,000 respondents. Moreover the WVS is the only academic study covering the full range of global variations, from very poor to very rich countries, in all of the world’s major cultural zones.</t>
+  </si>
+  <si>
+    <t>What is the aim of the World Value Survey?</t>
+  </si>
+  <si>
+    <t>The World Value Survey (WVS) seeks to help scientists and policy makers understand changes in the beliefs, values and motivations of people throughout the world. Thousands of political scientists, sociologists, social psychologists, anthropologists and economists have used these data to analyze such topics as economic development, democratization, religion, gender equality, social capital, and subjective well-being. These data have also been widely used by government officials, journalists and students, and groups at the World Bank have analyzed the linkages between cultural factors and economic development.</t>
+  </si>
+  <si>
+    <t>How can the information collected be used?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please explain what is meant by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Traditional values versus Secular-rational values"?</t>
+    </r>
+  </si>
+  <si>
+    <t>What does "Survival values versus Self-expression values" refer to?</t>
+  </si>
+  <si>
+    <t>What is meant by "Neutrality" in this context?</t>
+  </si>
+  <si>
+    <t>How is the "Fairness" value defined?</t>
+  </si>
+  <si>
+    <t>What does "Long- versus Short-Term Orientation" refer to in the context of the World Value Survey?</t>
+  </si>
+  <si>
+    <t>How is "Religiosity" defined in the context of analysing the World Value Survey?</t>
+  </si>
+  <si>
+    <t>Traditional values emphasize the importance of religion, parent-child ties, deference to authority and traditional family values. People who embrace these values also reject divorce, abortion, euthanasia and suicide. These societies have high levels of national pride and a nationalistic outlook.
+Secular-rational values have the opposite preferences to the traditional values. These societies place less emphasis on religion, traditional family values and authority. Divorce, abortion, euthanasia and suicide are seen as relatively acceptable, however suicide is not necessarily more common.</t>
+  </si>
+  <si>
+    <t>Survival values place emphasis on economic and physical security. It is linked with a relatively ethnocentric outlook and low levels of trust and tolerance.
+Self-expression values give high priority to environmental protection, growing tolerance of foreigners, gays and lesbians and gender equality, and rising demands for participation in decision-making in economic and political life.</t>
+  </si>
+  <si>
+    <t>In the context of the World Value Survey (WVS) "Religiosity" represents a strong dedication to God and religious customs, but not any particular religious denomination. This dimension focuses on foundational moral values that historically have been held by religious leaders and texts. 
+Examples of the WVS questions include disapproval of divorce and homosexuality, opposition to abortion, the belief that religion is always right, the belief that religious leaders should be a part of the government, as well as confidence, membership and attendance in religious groups. 
+People in countries that score highly in "Religiosity" tend to be more traditional in following religious customs and beliefs while people in countries with low scores tend to be more accepting of secular and alternative lifestyle choices.</t>
+  </si>
+  <si>
+    <t>“Neutrality” is represented by questions related to membership (or lack thereof) in various types of organizations as well as participation in political activities. Neutrality represents low engagement with both civic engagement groups as well as individual needs or interest groups. Questions that relate at “Neutrality” include non-membership in environmental organizations, self-help groups, political parties and sports organizations. Neutrality also includes a lack of motivation to become involved in civic or political issues with the questions about participation in boycotts, strikes, and petitions. In the highest scoring countries, over 95% of the population are not in social organizations such as environmental organizations, humanitarian or charitable organizations. Neutrality therefore represents a lack of engagement and relevance of such activities. Countries with low Neutrality scores have more participation and therefore voluntary organizations have more relevance in these countries. Still, it is important to note that even low scoring countries have just half to one-third of its citizens in these social groups.</t>
+  </si>
+  <si>
+    <t>“Fairness” relates to how participants answered questions about where actions such as stealing, bribery, and violence are ever justifiable, despite the fact that these are illegal in the majority of justice systems. Theoretically, fairness is associated with a judgment of a social situation that creates cooperative behaviours; it can be used both proactively to create cooperative behaviours or reflectively to judge previous actions. The “Fairness” values does not define what constitutes stealing, bribery, or violent actions; however, it does identify the importance a society places on avoiding such behaviours as they are locally defined. The countries with high scores for “Fairness” have more than 85% of the population stating that it is never justifiable to do these things. Countries that have lower scores for “Fairness”, meaning approximately 50% of the population believe that it is never justifiable to do things like stealing, bribery, or violence.</t>
+  </si>
+  <si>
+    <t>What is meant by the value of "Scepticism"?</t>
+  </si>
+  <si>
+    <t>The “Scepticism” value aims to measures the lack of confidence in large organizations and institutions. Scepticism specifically identifies an unwillingness to give organizations, political or civic, the benefit of the doubt. Scepticism is considered a vital part of a democracy because it ensures that people continue to stay involved with elections and decisions made by the government. Scepticism holds organizations accountable by other organizations as well as court systems. A very high scepticism score implies that large proportions of the population (30% or more) tend to have relatively less confidence in their major institutions such as government groups, labour unions, press, and major corporations. On the other hand, in countries that have much lower Scepticism scores over 70% of the population have relatively more confidence in institutions.</t>
+  </si>
+  <si>
+    <t>How is "Societal Tranquillity" defined?</t>
+  </si>
+  <si>
+    <t>“Societal Tranquillity” measures the lack of worry related to societal events and conversely the importance of peacefulness. Worrying is a symptom of anxiety due to uncertainty and how comfortable societies are with these uncertainties. Some worries are associated with circumstances such as civil war that may be out of respondent’s control and are therefore experienced at the societal level. Therefore, worrying can be imposed at the societal level. Societal Tranquillity is peace of mind that people have learned to value such that people feel safe, calm, and harmony in the same way across countries. In countries where approximately half of the responses indicated that they worry very little about war, terrorism, spying, employment, or education for their children score highly in “Societal Tranquillity”. On the other hand, in countries that score low for this value respondents are mainly worried about war, terrorism, employment and education. It is worth noting that historical and current situations (i.e. civil war, economic growth) within a country undoubtedly provide substantial context for the concerns in this dimension; nevertheless, it is still a social value if societies worry about these situations.</t>
+  </si>
+  <si>
+    <t>The Wold Value Survey (WVS) provides empirical evidence of cultural change and the persistence of distinctive cultural traditions. Analysis of WVS data made by political scientists Ronald Inglehart and Christian Welzel suggests that socioeconomic development is linked with a broad syndrome of distinctive value orientations. In their research they identify two major dimensions of cross cultural variation in the world, namely "Traditional values versus Secular-rational values" and "Survival values versus Self-expression values". Researchers have also indentified "Religiosity", "Neutrality", "Fairness", "Scepticism", "Societal Tranquillity" and "Long- versus Short-Term Orientation" as other values of potential interest.</t>
+  </si>
+  <si>
+    <t>The “long- versus short-term orientation” refers to whether a society exhibits a pragmatic future-oriented perspective or a conventional historic point of view. Long Term Orientation stands for the fostering of virtues oriented towards future rewards, in particular, perseverance and thrift. Its opposite pole Short-Term Orientation stands for the fostering of virtues related to the past and present, respect for tradition, preservation of 'face,' and fulfilling social obligations. A Long-Term Orientation is characterised by an emphasis on persistence, relationships being ordered by status, importance placed in personal adaptability, lower emphasis on leisure time, valuing of relationships and market positions and the belief that good or evil depends on the circumstances. One the other hand, Short-Term Orientation is characterised by an emphasis on quick results, status not a being major issue in relationships, valuing of personal steadfastness and stability, importance of leisure time and belief in absolutes about good and evil.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -173,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -194,6 +287,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1326,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E980"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1353,7 +1452,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="6"/>
@@ -1361,78 +1460,122 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="60.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="30.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="30.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" ht="30.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="45.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" ht="45.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="90.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="45.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="45.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="90.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="60.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
+      <c r="A13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>

</xml_diff>